<commit_message>
Batch Ed's MBLD result to be DNF
</commit_message>
<xml_diff>
--- a/data/2022-05-02/SCW Weekly Comp 2022-05-02 (Responses).xlsx
+++ b/data/2022-05-02/SCW Weekly Comp 2022-05-02 (Responses).xlsx
@@ -1,12 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwgeo\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C1EB3D-DDF0-4BBA-ACCF-AFA5A373C099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Form responses 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Form responses 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Form responses 1'!$A$1:$DF$50</definedName>
+  </definedNames>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -589,25 +601,28 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -615,7 +630,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -625,45 +640,44 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -853,26 +867,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:DF50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="CS1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="DD33" sqref="DD33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="116" width="18.88"/>
+    <col min="1" max="116" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1204,9 +1221,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>44685.23429384259</v>
+        <v>44685.234293842594</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>19</v>
@@ -1224,24 +1241,24 @@
         <v>23</v>
       </c>
       <c r="CJ2" s="3">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="CK2" s="3">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="CL2" s="3">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="CM2" s="3">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="CN2" s="3">
         <v>27.33</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>44685.66876782407</v>
+        <v>44685.668767824071</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>24</v>
@@ -1283,9 +1300,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>44685.68593571759</v>
+        <v>44685.685935717593</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>24</v>
@@ -1324,9 +1341,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>44688.75003921296</v>
+        <v>44688.750039212959</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>44</v>
@@ -1350,7 +1367,7 @@
         <v>9.31</v>
       </c>
       <c r="K5" s="3">
-        <v>8.88</v>
+        <v>8.8800000000000008</v>
       </c>
       <c r="L5" s="3">
         <v>5.01</v>
@@ -1362,9 +1379,9 @@
         <v>8.59</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>44689.70080733796</v>
+        <v>44689.700807337962</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>44</v>
@@ -1391,7 +1408,7 @@
         <v>6.61</v>
       </c>
       <c r="BL6" s="3">
-        <v>8.78</v>
+        <v>8.7799999999999994</v>
       </c>
       <c r="BM6" s="3">
         <v>6.61</v>
@@ -1400,9 +1417,9 @@
         <v>9.83</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>44690.62125809028</v>
+        <v>44690.621258090279</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>50</v>
@@ -1429,7 +1446,7 @@
         <v>22.69</v>
       </c>
       <c r="R7" s="3">
-        <v>19.24</v>
+        <v>19.239999999999998</v>
       </c>
       <c r="S7" s="3">
         <v>24.59</v>
@@ -1441,9 +1458,9 @@
         <v>20.43</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>44690.62215701389</v>
+        <v>44690.622157013888</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>50</v>
@@ -1482,9 +1499,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>44690.62320460648</v>
+        <v>44690.623204606483</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>50</v>
@@ -1523,9 +1540,9 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>44690.6238697338</v>
+        <v>44690.623869733798</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>50</v>
@@ -1558,7 +1575,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44690.624537766205</v>
       </c>
@@ -1593,9 +1610,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>44690.85183770834</v>
+        <v>44690.851837708338</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>80</v>
@@ -1631,9 +1648,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>44690.85455938657</v>
+        <v>44690.854559386571</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>80</v>
@@ -1669,9 +1686,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>44694.51043913195</v>
+        <v>44694.510439131947</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>96</v>
@@ -1689,7 +1706,7 @@
         <v>98</v>
       </c>
       <c r="CJ14" s="3">
-        <v>52.0</v>
+        <v>52</v>
       </c>
       <c r="CK14" s="3" t="s">
         <v>99</v>
@@ -1698,13 +1715,13 @@
         <v>99</v>
       </c>
       <c r="CM14" s="3">
-        <v>52.0</v>
+        <v>52</v>
       </c>
       <c r="CN14" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>44695.194557442126</v>
       </c>
@@ -1745,9 +1762,9 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>44695.19564348379</v>
+        <v>44695.195643483792</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>100</v>
@@ -1768,7 +1785,7 @@
         <v>19.3</v>
       </c>
       <c r="BP16" s="3">
-        <v>18.83</v>
+        <v>18.829999999999998</v>
       </c>
       <c r="BQ16" s="3">
         <v>14.72</v>
@@ -1783,12 +1800,12 @@
         <v>14.72</v>
       </c>
       <c r="BU16" s="3">
-        <v>18.51</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>18.510000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:97" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>44695.19648863426</v>
+        <v>44695.196488634261</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>100</v>
@@ -1827,9 +1844,9 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:97" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>44695.69190369213</v>
+        <v>44695.691903692132</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>112</v>
@@ -1868,9 +1885,9 @@
         <v>24.24</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:97" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>44695.69377201389</v>
+        <v>44695.693772013889</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>112</v>
@@ -1909,7 +1926,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:97" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>44695.695143854166</v>
       </c>
@@ -1950,9 +1967,9 @@
         <v>11.59</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:97" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>44695.69777804398</v>
+        <v>44695.697778043977</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>112</v>
@@ -1970,7 +1987,7 @@
         <v>115</v>
       </c>
       <c r="H21" s="3">
-        <v>8.29</v>
+        <v>8.2899999999999991</v>
       </c>
       <c r="I21" s="3">
         <v>5.82</v>
@@ -1979,7 +1996,7 @@
         <v>8.18</v>
       </c>
       <c r="K21" s="3">
-        <v>8.95</v>
+        <v>8.9499999999999993</v>
       </c>
       <c r="L21" s="3">
         <v>11.9</v>
@@ -1988,12 +2005,12 @@
         <v>5.82</v>
       </c>
       <c r="N21" s="5">
-        <v>8.47</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>8.4700000000000006</v>
+      </c>
+    </row>
+    <row r="22" spans="1:97" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>44695.69897880787</v>
+        <v>44695.698978807872</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>112</v>
@@ -2032,9 +2049,9 @@
         <v>27.43</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:97" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>44695.70051769676</v>
+        <v>44695.700517696758</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>112</v>
@@ -2073,7 +2090,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:97" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>44695.701853252314</v>
       </c>
@@ -2114,9 +2131,9 @@
         <v>126</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:97" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>44696.20084952546</v>
+        <v>44696.200849525463</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>127</v>
@@ -2155,7 +2172,7 @@
         <v>7.55</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:97" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>44696.20223490741</v>
       </c>
@@ -2196,9 +2213,9 @@
         <v>21.71</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:97" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>44696.20353297454</v>
+        <v>44696.203532974541</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>130</v>
@@ -2216,7 +2233,7 @@
         <v>132</v>
       </c>
       <c r="BV27" s="3">
-        <v>34.34</v>
+        <v>34.340000000000003</v>
       </c>
       <c r="BW27" s="3">
         <v>34.42</v>
@@ -2234,10 +2251,10 @@
         <v>29.47</v>
       </c>
       <c r="CB27" s="3">
-        <v>32.91</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>32.909999999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:97" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>44696.204593229166</v>
       </c>
@@ -2278,9 +2295,9 @@
         <v>15.07</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:97" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>44696.2928991088</v>
+        <v>44696.292899108797</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>134</v>
@@ -2307,7 +2324,7 @@
         <v>21.34</v>
       </c>
       <c r="R29" s="3">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="S29" s="3">
         <v>18.5</v>
@@ -2319,9 +2336,9 @@
         <v>21.01</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:97" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>44696.40461315972</v>
+        <v>44696.404613159721</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>134</v>
@@ -2354,7 +2371,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:97" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>44696.683748958334</v>
       </c>
@@ -2395,9 +2412,9 @@
         <v>15.13</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:97" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>44696.6845475463</v>
+        <v>44696.684547546298</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>140</v>
@@ -2430,9 +2447,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>44696.68586017361</v>
+        <v>44696.685860173609</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>140</v>
@@ -2450,16 +2467,16 @@
         <v>147</v>
       </c>
       <c r="DD33" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="DE33" s="5">
-        <v>1.0</v>
+        <v>0</v>
       </c>
       <c r="DF33" s="6" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>44696.696928391204</v>
       </c>
@@ -2500,7 +2517,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>44696.699156331015</v>
       </c>
@@ -2541,9 +2558,9 @@
         <v>160</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>44696.70164002315</v>
+        <v>44696.701640023151</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>149</v>
@@ -2579,12 +2596,12 @@
         <v>31.35</v>
       </c>
       <c r="U36" s="3">
-        <v>40.73</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>40.729999999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>44696.7220291088</v>
+        <v>44696.722029108802</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>100</v>
@@ -2623,9 +2640,9 @@
         <v>27.31</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>44696.72268465278</v>
+        <v>44696.722684652777</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>100</v>
@@ -2664,9 +2681,9 @@
         <v>7.63</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>44696.74266962963</v>
+        <v>44696.742669629632</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>100</v>
@@ -2705,7 +2722,7 @@
         <v>11.48</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>44696.80438987269</v>
       </c>
@@ -2728,7 +2745,7 @@
         <v>45.81</v>
       </c>
       <c r="BW40" s="3">
-        <v>47.0</v>
+        <v>47</v>
       </c>
       <c r="BX40" s="3" t="s">
         <v>168</v>
@@ -2746,9 +2763,9 @@
         <v>48.99</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>44696.80545546296</v>
+        <v>44696.805455462963</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>165</v>
@@ -2775,7 +2792,7 @@
         <v>18.96</v>
       </c>
       <c r="BR41" s="3">
-        <v>18.15</v>
+        <v>18.149999999999999</v>
       </c>
       <c r="BS41" s="3">
         <v>30.02</v>
@@ -2784,12 +2801,12 @@
         <v>15.31</v>
       </c>
       <c r="BU41" s="3">
-        <v>20.08</v>
-      </c>
-    </row>
-    <row r="42">
+        <v>20.079999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>44696.80657059028</v>
+        <v>44696.806570590277</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>165</v>
@@ -2828,9 +2845,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>44696.80782886574</v>
+        <v>44696.807828865742</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>165</v>
@@ -2869,9 +2886,9 @@
         <v>179</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>44696.8090465625</v>
+        <v>44696.809046562499</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>165</v>
@@ -2901,7 +2918,7 @@
         <v>33.35</v>
       </c>
       <c r="S44" s="3">
-        <v>32.66</v>
+        <v>32.659999999999997</v>
       </c>
       <c r="T44" s="3">
         <v>27.45</v>
@@ -2910,9 +2927,9 @@
         <v>34.35</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>44696.81009475695</v>
+        <v>44696.810094756947</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>165</v>
@@ -2951,9 +2968,9 @@
         <v>9.44</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>44696.98783783565</v>
+        <v>44696.987837835652</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>149</v>
@@ -2974,10 +2991,10 @@
         <v>11.32</v>
       </c>
       <c r="I46" s="3">
-        <v>8.55</v>
+        <v>8.5500000000000007</v>
       </c>
       <c r="J46" s="3">
-        <v>8.97</v>
+        <v>8.9700000000000006</v>
       </c>
       <c r="K46" s="3">
         <v>8.07</v>
@@ -2992,7 +3009,7 @@
         <v>9.39</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>44697.00197975694</v>
       </c>
@@ -3033,9 +3050,9 @@
         <v>11.48</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:110" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>44697.02056917824</v>
+        <v>44697.020569178239</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>149</v>
@@ -3065,18 +3082,18 @@
         <v>13.37</v>
       </c>
       <c r="BL48" s="3">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="BM48" s="3">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="BN48" s="3">
         <v>13.45</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:87" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>44697.02435974537</v>
+        <v>44697.024359745366</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>149</v>
@@ -3115,7 +3132,7 @@
         <v>26.39</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:87" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>44697.05297153935</v>
       </c>
@@ -3157,57 +3174,64 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:DF50" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="3x3x3 Multi-Blind"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F2"/>
-    <hyperlink r:id="rId2" ref="F3"/>
-    <hyperlink r:id="rId3" ref="F4"/>
-    <hyperlink r:id="rId4" ref="F5"/>
-    <hyperlink r:id="rId5" ref="F6"/>
-    <hyperlink r:id="rId6" ref="F7"/>
-    <hyperlink r:id="rId7" ref="F8"/>
-    <hyperlink r:id="rId8" ref="F9"/>
-    <hyperlink r:id="rId9" ref="F10"/>
-    <hyperlink r:id="rId10" ref="F11"/>
-    <hyperlink r:id="rId11" ref="F12"/>
-    <hyperlink r:id="rId12" ref="F13"/>
-    <hyperlink r:id="rId13" ref="F14"/>
-    <hyperlink r:id="rId14" ref="F15"/>
-    <hyperlink r:id="rId15" ref="F16"/>
-    <hyperlink r:id="rId16" ref="F17"/>
-    <hyperlink r:id="rId17" ref="F18"/>
-    <hyperlink r:id="rId18" ref="F19"/>
-    <hyperlink r:id="rId19" ref="F20"/>
-    <hyperlink r:id="rId20" ref="F21"/>
-    <hyperlink r:id="rId21" ref="F22"/>
-    <hyperlink r:id="rId22" ref="F23"/>
-    <hyperlink r:id="rId23" ref="F24"/>
-    <hyperlink r:id="rId24" ref="F25"/>
-    <hyperlink r:id="rId25" ref="F26"/>
-    <hyperlink r:id="rId26" ref="F27"/>
-    <hyperlink r:id="rId27" ref="F28"/>
-    <hyperlink r:id="rId28" ref="F29"/>
-    <hyperlink r:id="rId29" ref="F30"/>
-    <hyperlink r:id="rId30" ref="F31"/>
-    <hyperlink r:id="rId31" ref="F32"/>
-    <hyperlink r:id="rId32" ref="F33"/>
-    <hyperlink r:id="rId33" ref="F34"/>
-    <hyperlink r:id="rId34" ref="F35"/>
-    <hyperlink r:id="rId35" ref="F36"/>
-    <hyperlink r:id="rId36" ref="F37"/>
-    <hyperlink r:id="rId37" ref="F38"/>
-    <hyperlink r:id="rId38" ref="F39"/>
-    <hyperlink r:id="rId39" ref="F40"/>
-    <hyperlink r:id="rId40" ref="F41"/>
-    <hyperlink r:id="rId41" ref="F42"/>
-    <hyperlink r:id="rId42" ref="F43"/>
-    <hyperlink r:id="rId43" ref="F44"/>
-    <hyperlink r:id="rId44" ref="F45"/>
-    <hyperlink r:id="rId45" ref="F46"/>
-    <hyperlink r:id="rId46" ref="F47"/>
-    <hyperlink r:id="rId47" ref="F48"/>
-    <hyperlink r:id="rId48" ref="F49"/>
-    <hyperlink r:id="rId49" ref="F50"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="F15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="F16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="F17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="F18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="F19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="F21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="F22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="F23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="F24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="F25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="F26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="F27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="F28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="F29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="F30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="F31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="F32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="F33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="F34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="F35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="F36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="F37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="F38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="F39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="F40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="F41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="F42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="F43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="F44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="F45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="F46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="F47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="F48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="F49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="F50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
   </hyperlinks>
-  <drawing r:id="rId50"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>